<commit_message>
Laravel setup for manage xlsx data
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp_v8.1.1\htdocs\xlsx-reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4111487-76F7-4847-BCA6-15F7E40BFBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFF9C73-A398-4AA4-A1DF-08668900D514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="5760" windowWidth="24210" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="3330" windowWidth="24210" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -596,11 +596,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -909,7 +911,7 @@
   <dimension ref="A1:DE441"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="K2" sqref="K2:K441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +926,7 @@
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
@@ -974,7 +976,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1057,7 +1059,7 @@
       <c r="J2">
         <v>2</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="5">
         <v>40</v>
       </c>
       <c r="L2">
@@ -1137,7 +1139,7 @@
       <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="5">
         <v>45</v>
       </c>
       <c r="L3">
@@ -1214,7 +1216,7 @@
       <c r="J4">
         <v>2</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="5">
         <v>45</v>
       </c>
       <c r="L4">
@@ -1291,7 +1293,7 @@
       <c r="J5">
         <v>2</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <v>45</v>
       </c>
       <c r="L5">
@@ -1368,7 +1370,7 @@
       <c r="J6">
         <v>2</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <v>45</v>
       </c>
       <c r="L6">
@@ -1445,7 +1447,7 @@
       <c r="J7">
         <v>2</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>50</v>
       </c>
       <c r="L7">
@@ -1522,7 +1524,7 @@
       <c r="J8">
         <v>2</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="5">
         <v>53</v>
       </c>
       <c r="L8">
@@ -1599,7 +1601,7 @@
       <c r="J9">
         <v>2</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="5">
         <v>55</v>
       </c>
       <c r="L9">
@@ -1676,7 +1678,7 @@
       <c r="J10">
         <v>2</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="5">
         <v>55</v>
       </c>
       <c r="L10">
@@ -1753,7 +1755,7 @@
       <c r="J11">
         <v>2</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="5">
         <v>55</v>
       </c>
       <c r="L11">
@@ -1830,7 +1832,7 @@
       <c r="J12">
         <v>2</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <v>40</v>
       </c>
       <c r="L12">
@@ -1907,7 +1909,7 @@
       <c r="J13">
         <v>2</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="5">
         <v>60</v>
       </c>
       <c r="L13">
@@ -1984,7 +1986,7 @@
       <c r="J14">
         <v>2</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="5">
         <v>60</v>
       </c>
       <c r="L14">
@@ -2061,7 +2063,7 @@
       <c r="J15">
         <v>2</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="5">
         <v>65</v>
       </c>
       <c r="L15">
@@ -2138,7 +2140,7 @@
       <c r="J16">
         <v>2</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="5">
         <v>69</v>
       </c>
       <c r="L16">
@@ -2215,7 +2217,7 @@
       <c r="J17">
         <v>2</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="5">
         <v>70</v>
       </c>
       <c r="L17">
@@ -2292,7 +2294,7 @@
       <c r="J18">
         <v>2</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="5">
         <v>70</v>
       </c>
       <c r="L18">
@@ -2369,7 +2371,7 @@
       <c r="J19">
         <v>2</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="5">
         <v>70</v>
       </c>
       <c r="L19">
@@ -2446,7 +2448,7 @@
       <c r="J20">
         <v>2</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="5">
         <v>72</v>
       </c>
       <c r="L20">
@@ -2523,7 +2525,7 @@
       <c r="J21">
         <v>2</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="5">
         <v>75</v>
       </c>
       <c r="L21">
@@ -2603,7 +2605,7 @@
       <c r="J22">
         <v>2</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="5">
         <v>75</v>
       </c>
       <c r="L22">
@@ -2680,7 +2682,7 @@
       <c r="J23">
         <v>2</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="5">
         <v>80</v>
       </c>
       <c r="L23">
@@ -2757,7 +2759,7 @@
       <c r="J24">
         <v>2</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="5">
         <v>80</v>
       </c>
       <c r="L24">
@@ -2834,7 +2836,7 @@
       <c r="J25">
         <v>2</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="5">
         <v>80</v>
       </c>
       <c r="L25">
@@ -2911,7 +2913,7 @@
       <c r="J26">
         <v>2</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="5">
         <v>85</v>
       </c>
       <c r="L26">
@@ -2988,7 +2990,7 @@
       <c r="J27">
         <v>2</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="5">
         <v>85</v>
       </c>
       <c r="L27">
@@ -3065,7 +3067,7 @@
       <c r="J28">
         <v>2</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="5">
         <v>85</v>
       </c>
       <c r="L28">
@@ -3142,7 +3144,7 @@
       <c r="J29">
         <v>2</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="5">
         <v>135</v>
       </c>
       <c r="L29">
@@ -3219,7 +3221,7 @@
       <c r="J30">
         <v>0</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="5">
         <v>23</v>
       </c>
       <c r="L30">
@@ -3296,7 +3298,7 @@
       <c r="J31">
         <v>2</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="5">
         <v>85</v>
       </c>
       <c r="L31">
@@ -3373,7 +3375,7 @@
       <c r="J32">
         <v>2</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="5">
         <v>85</v>
       </c>
       <c r="L32">
@@ -3450,7 +3452,7 @@
       <c r="J33">
         <v>2</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="5">
         <v>95</v>
       </c>
       <c r="L33">
@@ -3527,7 +3529,7 @@
       <c r="J34">
         <v>2</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="5">
         <v>98</v>
       </c>
       <c r="L34">
@@ -3604,7 +3606,7 @@
       <c r="J35">
         <v>2</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="5">
         <v>100</v>
       </c>
       <c r="L35">
@@ -3681,7 +3683,7 @@
       <c r="J36">
         <v>2</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="5">
         <v>100</v>
       </c>
       <c r="L36">
@@ -3758,7 +3760,7 @@
       <c r="J37">
         <v>2</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="5">
         <v>100</v>
       </c>
       <c r="L37">
@@ -3835,7 +3837,7 @@
       <c r="J38">
         <v>2</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="5">
         <v>58</v>
       </c>
       <c r="L38">
@@ -3912,7 +3914,7 @@
       <c r="J39">
         <v>2</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="5">
         <v>100</v>
       </c>
       <c r="L39">
@@ -3989,7 +3991,7 @@
       <c r="J40">
         <v>2</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="5">
         <v>100</v>
       </c>
       <c r="L40">
@@ -4066,7 +4068,7 @@
       <c r="J41">
         <v>2</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="5">
         <v>100</v>
       </c>
       <c r="L41">
@@ -4143,7 +4145,7 @@
       <c r="J42">
         <v>2</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="5">
         <v>100</v>
       </c>
       <c r="L42">
@@ -4220,7 +4222,7 @@
       <c r="J43">
         <v>2</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="5">
         <v>105</v>
       </c>
       <c r="L43">
@@ -4297,7 +4299,7 @@
       <c r="J44">
         <v>2</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="5">
         <v>110</v>
       </c>
       <c r="L44">
@@ -4374,7 +4376,7 @@
       <c r="J45">
         <v>2</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="5">
         <v>115</v>
       </c>
       <c r="L45">
@@ -4451,7 +4453,7 @@
       <c r="J46">
         <v>2</v>
       </c>
-      <c r="K46">
+      <c r="K46" s="5">
         <v>120</v>
       </c>
       <c r="L46">
@@ -4528,7 +4530,7 @@
       <c r="J47">
         <v>0.5</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="5">
         <v>120</v>
       </c>
       <c r="L47">
@@ -4605,7 +4607,7 @@
       <c r="J48">
         <v>2</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="5">
         <v>50</v>
       </c>
       <c r="L48">
@@ -4682,7 +4684,7 @@
       <c r="J49">
         <v>2</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="5">
         <v>135</v>
       </c>
       <c r="L49">
@@ -4759,7 +4761,7 @@
       <c r="J50">
         <v>2</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="5">
         <v>140</v>
       </c>
       <c r="L50">
@@ -4836,7 +4838,7 @@
       <c r="J51">
         <v>2</v>
       </c>
-      <c r="K51">
+      <c r="K51" s="5">
         <v>140</v>
       </c>
       <c r="L51">
@@ -4913,7 +4915,7 @@
       <c r="J52">
         <v>2</v>
       </c>
-      <c r="K52">
+      <c r="K52" s="5">
         <v>140</v>
       </c>
       <c r="L52">
@@ -4990,7 +4992,7 @@
       <c r="J53">
         <v>2</v>
       </c>
-      <c r="K53">
+      <c r="K53" s="5">
         <v>145</v>
       </c>
       <c r="L53">
@@ -5067,7 +5069,7 @@
       <c r="J54">
         <v>2</v>
       </c>
-      <c r="K54">
+      <c r="K54" s="5">
         <v>145</v>
       </c>
       <c r="L54">
@@ -5147,7 +5149,7 @@
       <c r="J55">
         <v>2</v>
       </c>
-      <c r="K55">
+      <c r="K55" s="5">
         <v>150</v>
       </c>
       <c r="L55">
@@ -5224,7 +5226,7 @@
       <c r="J56">
         <v>2</v>
       </c>
-      <c r="K56">
+      <c r="K56" s="5">
         <v>150</v>
       </c>
       <c r="L56">
@@ -5301,7 +5303,7 @@
       <c r="J57">
         <v>2</v>
       </c>
-      <c r="K57">
+      <c r="K57" s="5">
         <v>150</v>
       </c>
       <c r="L57">
@@ -5381,7 +5383,7 @@
       <c r="J58">
         <v>2</v>
       </c>
-      <c r="K58">
+      <c r="K58" s="5">
         <v>160</v>
       </c>
       <c r="L58">
@@ -5458,7 +5460,7 @@
       <c r="J59">
         <v>2</v>
       </c>
-      <c r="K59">
+      <c r="K59" s="5">
         <v>170</v>
       </c>
       <c r="L59">
@@ -5535,7 +5537,7 @@
       <c r="J60">
         <v>2</v>
       </c>
-      <c r="K60">
+      <c r="K60" s="5">
         <v>200</v>
       </c>
       <c r="L60">
@@ -5612,7 +5614,7 @@
       <c r="J61">
         <v>2</v>
       </c>
-      <c r="K61">
+      <c r="K61" s="5">
         <v>210</v>
       </c>
       <c r="L61">
@@ -5689,7 +5691,7 @@
       <c r="J62">
         <v>2</v>
       </c>
-      <c r="K62">
+      <c r="K62" s="5">
         <v>210</v>
       </c>
       <c r="L62">
@@ -5766,7 +5768,7 @@
       <c r="J63">
         <v>2</v>
       </c>
-      <c r="K63">
+      <c r="K63" s="5">
         <v>210</v>
       </c>
       <c r="L63">
@@ -5843,7 +5845,7 @@
       <c r="J64">
         <v>2</v>
       </c>
-      <c r="K64">
+      <c r="K64" s="5">
         <v>250</v>
       </c>
       <c r="L64">
@@ -5920,7 +5922,7 @@
       <c r="J65">
         <v>2</v>
       </c>
-      <c r="K65">
+      <c r="K65" s="5">
         <v>270</v>
       </c>
       <c r="L65">
@@ -5997,7 +5999,7 @@
       <c r="J66">
         <v>2</v>
       </c>
-      <c r="K66">
+      <c r="K66" s="5">
         <v>80</v>
       </c>
       <c r="L66">
@@ -6071,7 +6073,7 @@
       <c r="J67" t="s">
         <v>165</v>
       </c>
-      <c r="K67" t="s">
+      <c r="K67" s="5" t="s">
         <v>165</v>
       </c>
       <c r="L67" t="s">
@@ -6148,7 +6150,7 @@
       <c r="J68">
         <v>0.5</v>
       </c>
-      <c r="K68">
+      <c r="K68" s="5">
         <v>30</v>
       </c>
       <c r="L68">
@@ -6228,7 +6230,7 @@
       <c r="J69">
         <v>2</v>
       </c>
-      <c r="K69">
+      <c r="K69" s="5">
         <v>100</v>
       </c>
       <c r="L69">
@@ -6305,7 +6307,7 @@
       <c r="J70">
         <v>2</v>
       </c>
-      <c r="K70">
+      <c r="K70" s="5">
         <v>140</v>
       </c>
       <c r="L70">
@@ -6382,7 +6384,7 @@
       <c r="J71">
         <v>2</v>
       </c>
-      <c r="K71">
+      <c r="K71" s="5">
         <v>310</v>
       </c>
       <c r="L71">
@@ -6459,7 +6461,7 @@
       <c r="J72">
         <v>2</v>
       </c>
-      <c r="K72">
+      <c r="K72" s="5">
         <v>75</v>
       </c>
       <c r="L72">
@@ -6536,7 +6538,7 @@
       <c r="J73">
         <v>2</v>
       </c>
-      <c r="K73">
+      <c r="K73" s="5">
         <v>80</v>
       </c>
       <c r="L73">
@@ -6613,7 +6615,7 @@
       <c r="J74">
         <v>2</v>
       </c>
-      <c r="K74">
+      <c r="K74" s="5">
         <v>55</v>
       </c>
       <c r="L74">
@@ -6693,7 +6695,7 @@
       <c r="J75">
         <v>2</v>
       </c>
-      <c r="K75">
+      <c r="K75" s="5">
         <v>95</v>
       </c>
       <c r="L75">
@@ -6770,7 +6772,7 @@
       <c r="J76">
         <v>2</v>
       </c>
-      <c r="K76">
+      <c r="K76" s="5">
         <v>55</v>
       </c>
       <c r="L76">
@@ -6847,7 +6849,7 @@
       <c r="J77">
         <v>2</v>
       </c>
-      <c r="K77">
+      <c r="K77" s="5">
         <v>230</v>
       </c>
       <c r="L77">
@@ -6924,7 +6926,7 @@
       <c r="J78">
         <v>2</v>
       </c>
-      <c r="K78">
+      <c r="K78" s="5">
         <v>140</v>
       </c>
       <c r="L78">
@@ -7001,7 +7003,7 @@
       <c r="J79">
         <v>2</v>
       </c>
-      <c r="K79">
+      <c r="K79" s="5">
         <v>55</v>
       </c>
       <c r="L79">
@@ -7078,7 +7080,7 @@
       <c r="J80">
         <v>2</v>
       </c>
-      <c r="K80">
+      <c r="K80" s="5">
         <v>40</v>
       </c>
       <c r="L80">
@@ -7155,7 +7157,7 @@
       <c r="J81">
         <v>2</v>
       </c>
-      <c r="K81">
+      <c r="K81" s="5">
         <v>60</v>
       </c>
       <c r="L81">
@@ -7232,7 +7234,7 @@
       <c r="J82">
         <v>2</v>
       </c>
-      <c r="K82">
+      <c r="K82" s="5">
         <v>30</v>
       </c>
       <c r="L82">
@@ -7309,7 +7311,7 @@
       <c r="J83">
         <v>2</v>
       </c>
-      <c r="K83">
+      <c r="K83" s="5">
         <v>40</v>
       </c>
       <c r="L83">
@@ -7389,7 +7391,7 @@
       <c r="J84">
         <v>2</v>
       </c>
-      <c r="K84">
+      <c r="K84" s="5">
         <v>150</v>
       </c>
       <c r="L84">
@@ -7466,7 +7468,7 @@
       <c r="J85">
         <v>2</v>
       </c>
-      <c r="K85">
+      <c r="K85" s="5">
         <v>125</v>
       </c>
       <c r="L85">
@@ -7543,7 +7545,7 @@
       <c r="J86">
         <v>2</v>
       </c>
-      <c r="K86">
+      <c r="K86" s="5">
         <v>70</v>
       </c>
       <c r="L86">
@@ -7620,7 +7622,7 @@
       <c r="J87">
         <v>2</v>
       </c>
-      <c r="K87">
+      <c r="K87" s="5">
         <v>50</v>
       </c>
       <c r="L87">
@@ -7697,7 +7699,7 @@
       <c r="J88">
         <v>2</v>
       </c>
-      <c r="K88">
+      <c r="K88" s="5">
         <v>70</v>
       </c>
       <c r="L88">
@@ -7774,7 +7776,7 @@
       <c r="J89">
         <v>2</v>
       </c>
-      <c r="K89">
+      <c r="K89" s="5">
         <v>65</v>
       </c>
       <c r="L89">
@@ -7851,7 +7853,7 @@
       <c r="J90">
         <v>2</v>
       </c>
-      <c r="K90">
+      <c r="K90" s="5">
         <v>70</v>
       </c>
       <c r="L90">
@@ -7928,7 +7930,7 @@
       <c r="J91">
         <v>2</v>
       </c>
-      <c r="K91">
+      <c r="K91" s="5">
         <v>75</v>
       </c>
       <c r="L91">
@@ -8005,7 +8007,7 @@
       <c r="J92">
         <v>2</v>
       </c>
-      <c r="K92">
+      <c r="K92" s="5">
         <v>25</v>
       </c>
       <c r="L92">
@@ -8082,7 +8084,7 @@
       <c r="J93">
         <v>2</v>
       </c>
-      <c r="K93">
+      <c r="K93" s="5">
         <v>35</v>
       </c>
       <c r="L93">
@@ -8159,7 +8161,7 @@
       <c r="J94">
         <v>2</v>
       </c>
-      <c r="K94">
+      <c r="K94" s="5">
         <v>100</v>
       </c>
       <c r="L94">
@@ -8236,7 +8238,7 @@
       <c r="J95">
         <v>2</v>
       </c>
-      <c r="K95">
+      <c r="K95" s="5">
         <v>124</v>
       </c>
       <c r="L95">
@@ -8313,7 +8315,7 @@
       <c r="J96">
         <v>2</v>
       </c>
-      <c r="K96">
+      <c r="K96" s="5">
         <v>75</v>
       </c>
       <c r="L96">
@@ -8390,7 +8392,7 @@
       <c r="J97">
         <v>2</v>
       </c>
-      <c r="K97">
+      <c r="K97" s="5">
         <v>25</v>
       </c>
       <c r="L97">
@@ -8467,7 +8469,7 @@
       <c r="J98">
         <v>2</v>
       </c>
-      <c r="K98">
+      <c r="K98" s="5">
         <v>28</v>
       </c>
       <c r="L98">
@@ -8544,7 +8546,7 @@
       <c r="J99">
         <v>2</v>
       </c>
-      <c r="K99">
+      <c r="K99" s="5">
         <v>50</v>
       </c>
       <c r="L99">
@@ -8621,7 +8623,7 @@
       <c r="J100">
         <v>2</v>
       </c>
-      <c r="K100">
+      <c r="K100" s="5">
         <v>65</v>
       </c>
       <c r="L100">
@@ -8698,7 +8700,7 @@
       <c r="J101">
         <v>2</v>
       </c>
-      <c r="K101">
+      <c r="K101" s="5">
         <v>68</v>
       </c>
       <c r="L101">
@@ -8775,7 +8777,7 @@
       <c r="J102">
         <v>2</v>
       </c>
-      <c r="K102">
+      <c r="K102" s="5">
         <v>80</v>
       </c>
       <c r="L102">
@@ -8852,7 +8854,7 @@
       <c r="J103">
         <v>2</v>
       </c>
-      <c r="K103">
+      <c r="K103" s="5">
         <v>60</v>
       </c>
       <c r="L103">
@@ -8929,7 +8931,7 @@
       <c r="J104">
         <v>2</v>
       </c>
-      <c r="K104">
+      <c r="K104" s="5">
         <v>155</v>
       </c>
       <c r="L104">
@@ -9006,7 +9008,7 @@
       <c r="J105">
         <v>2</v>
       </c>
-      <c r="K105">
+      <c r="K105" s="5">
         <v>110</v>
       </c>
       <c r="L105">
@@ -9083,7 +9085,7 @@
       <c r="J106">
         <v>2</v>
       </c>
-      <c r="K106">
+      <c r="K106" s="5">
         <v>70</v>
       </c>
       <c r="L106">
@@ -9160,7 +9162,7 @@
       <c r="J107">
         <v>2</v>
       </c>
-      <c r="K107">
+      <c r="K107" s="5">
         <v>42</v>
       </c>
       <c r="L107">
@@ -9237,7 +9239,7 @@
       <c r="J108">
         <v>2</v>
       </c>
-      <c r="K108">
+      <c r="K108" s="5">
         <v>45</v>
       </c>
       <c r="L108">
@@ -9314,7 +9316,7 @@
       <c r="J109">
         <v>0.5</v>
       </c>
-      <c r="K109">
+      <c r="K109" s="5">
         <v>75</v>
       </c>
       <c r="L109">
@@ -9391,7 +9393,7 @@
       <c r="J110">
         <v>0.5</v>
       </c>
-      <c r="K110">
+      <c r="K110" s="5">
         <v>35</v>
       </c>
       <c r="L110">
@@ -9468,7 +9470,7 @@
       <c r="J111">
         <v>0.5</v>
       </c>
-      <c r="K111">
+      <c r="K111" s="5">
         <v>55</v>
       </c>
       <c r="L111">
@@ -9545,7 +9547,7 @@
       <c r="J112">
         <v>2</v>
       </c>
-      <c r="K112">
+      <c r="K112" s="5">
         <v>130</v>
       </c>
       <c r="L112">
@@ -9622,7 +9624,7 @@
       <c r="J113">
         <v>2</v>
       </c>
-      <c r="K113">
+      <c r="K113" s="5">
         <v>160</v>
       </c>
       <c r="L113">
@@ -9699,7 +9701,7 @@
       <c r="J114">
         <v>2</v>
       </c>
-      <c r="K114">
+      <c r="K114" s="5">
         <v>65</v>
       </c>
       <c r="L114">
@@ -9776,7 +9778,7 @@
       <c r="J115">
         <v>2</v>
       </c>
-      <c r="K115">
+      <c r="K115" s="5">
         <v>50</v>
       </c>
       <c r="L115">
@@ -9853,7 +9855,7 @@
       <c r="J116">
         <v>2</v>
       </c>
-      <c r="K116">
+      <c r="K116" s="5">
         <v>55</v>
       </c>
       <c r="L116">
@@ -9930,7 +9932,7 @@
       <c r="J117">
         <v>2</v>
       </c>
-      <c r="K117">
+      <c r="K117" s="5">
         <v>80</v>
       </c>
       <c r="L117">
@@ -10007,7 +10009,7 @@
       <c r="J118">
         <v>2</v>
       </c>
-      <c r="K118">
+      <c r="K118" s="5">
         <v>95</v>
       </c>
       <c r="L118">
@@ -10084,7 +10086,7 @@
       <c r="J119">
         <v>2</v>
       </c>
-      <c r="K119">
+      <c r="K119" s="5">
         <v>150</v>
       </c>
       <c r="L119">
@@ -10164,7 +10166,7 @@
       <c r="J120">
         <v>2</v>
       </c>
-      <c r="K120">
+      <c r="K120" s="5">
         <v>29</v>
       </c>
       <c r="L120">
@@ -10241,7 +10243,7 @@
       <c r="J121">
         <v>2</v>
       </c>
-      <c r="K121">
+      <c r="K121" s="5">
         <v>95</v>
       </c>
       <c r="L121">
@@ -10318,7 +10320,7 @@
       <c r="J122">
         <v>2</v>
       </c>
-      <c r="K122">
+      <c r="K122" s="5">
         <v>100</v>
       </c>
       <c r="L122">
@@ -10398,7 +10400,7 @@
       <c r="J123">
         <v>2</v>
       </c>
-      <c r="K123">
+      <c r="K123" s="5">
         <v>138</v>
       </c>
       <c r="L123">
@@ -10475,7 +10477,7 @@
       <c r="J124">
         <v>2</v>
       </c>
-      <c r="K124">
+      <c r="K124" s="5">
         <v>297</v>
       </c>
       <c r="L124">
@@ -10555,7 +10557,7 @@
       <c r="J125">
         <v>2</v>
       </c>
-      <c r="K125">
+      <c r="K125" s="5">
         <v>60</v>
       </c>
       <c r="L125">
@@ -10632,7 +10634,7 @@
       <c r="J126">
         <v>2</v>
       </c>
-      <c r="K126">
+      <c r="K126" s="5">
         <v>40</v>
       </c>
       <c r="L126">
@@ -10709,7 +10711,7 @@
       <c r="J127">
         <v>2</v>
       </c>
-      <c r="K127">
+      <c r="K127" s="5">
         <v>100</v>
       </c>
       <c r="L127">
@@ -10786,7 +10788,7 @@
       <c r="J128">
         <v>2</v>
       </c>
-      <c r="K128">
+      <c r="K128" s="5">
         <v>50</v>
       </c>
       <c r="L128">
@@ -10863,7 +10865,7 @@
       <c r="J129">
         <v>2</v>
       </c>
-      <c r="K129">
+      <c r="K129" s="5">
         <v>95</v>
       </c>
       <c r="L129">
@@ -10940,7 +10942,7 @@
       <c r="J130">
         <v>2.5</v>
       </c>
-      <c r="K130">
+      <c r="K130" s="5">
         <v>44</v>
       </c>
       <c r="L130">
@@ -11017,7 +11019,7 @@
       <c r="J131">
         <v>2</v>
       </c>
-      <c r="K131">
+      <c r="K131" s="5">
         <v>50</v>
       </c>
       <c r="L131">
@@ -11094,7 +11096,7 @@
       <c r="J132">
         <v>2</v>
       </c>
-      <c r="K132">
+      <c r="K132" s="5">
         <v>65</v>
       </c>
       <c r="L132">
@@ -11171,7 +11173,7 @@
       <c r="J133">
         <v>2</v>
       </c>
-      <c r="K133">
+      <c r="K133" s="5">
         <v>95</v>
       </c>
       <c r="L133">
@@ -11248,7 +11250,7 @@
       <c r="J134">
         <v>2</v>
       </c>
-      <c r="K134">
+      <c r="K134" s="5">
         <v>135</v>
       </c>
       <c r="L134">
@@ -11328,7 +11330,7 @@
       <c r="J135">
         <v>2</v>
       </c>
-      <c r="K135">
+      <c r="K135" s="5">
         <v>70</v>
       </c>
       <c r="L135">
@@ -11405,7 +11407,7 @@
       <c r="J136">
         <v>2</v>
       </c>
-      <c r="K136">
+      <c r="K136" s="5">
         <v>22</v>
       </c>
       <c r="L136">
@@ -11482,7 +11484,7 @@
       <c r="J137">
         <v>2</v>
       </c>
-      <c r="K137">
+      <c r="K137" s="5">
         <v>30</v>
       </c>
       <c r="L137">
@@ -11559,7 +11561,7 @@
       <c r="J138">
         <v>2</v>
       </c>
-      <c r="K138">
+      <c r="K138" s="5">
         <v>16</v>
       </c>
       <c r="L138">
@@ -11636,7 +11638,7 @@
       <c r="J139">
         <v>2</v>
       </c>
-      <c r="K139">
+      <c r="K139" s="5">
         <v>60</v>
       </c>
       <c r="L139">
@@ -11713,7 +11715,7 @@
       <c r="J140">
         <v>2</v>
       </c>
-      <c r="K140">
+      <c r="K140" s="5">
         <v>48</v>
       </c>
       <c r="L140">
@@ -11793,7 +11795,7 @@
       <c r="J141">
         <v>2</v>
       </c>
-      <c r="K141">
+      <c r="K141" s="5">
         <v>95</v>
       </c>
       <c r="L141">
@@ -11870,7 +11872,7 @@
       <c r="J142">
         <v>2</v>
       </c>
-      <c r="K142">
+      <c r="K142" s="5">
         <v>55</v>
       </c>
       <c r="L142">
@@ -11947,7 +11949,7 @@
       <c r="J143">
         <v>2</v>
       </c>
-      <c r="K143">
+      <c r="K143" s="5">
         <v>80</v>
       </c>
       <c r="L143">
@@ -12024,7 +12026,7 @@
       <c r="J144">
         <v>2</v>
       </c>
-      <c r="K144">
+      <c r="K144" s="5">
         <v>110</v>
       </c>
       <c r="L144">
@@ -12101,7 +12103,7 @@
       <c r="J145">
         <v>2</v>
       </c>
-      <c r="K145">
+      <c r="K145" s="5">
         <v>70</v>
       </c>
       <c r="L145">
@@ -12178,7 +12180,7 @@
       <c r="J146">
         <v>2</v>
       </c>
-      <c r="K146">
+      <c r="K146" s="5">
         <v>80</v>
       </c>
       <c r="L146">
@@ -12255,7 +12257,7 @@
       <c r="J147">
         <v>2</v>
       </c>
-      <c r="K147">
+      <c r="K147" s="5">
         <v>70</v>
       </c>
       <c r="L147">
@@ -12335,7 +12337,7 @@
       <c r="J148">
         <v>2</v>
       </c>
-      <c r="K148">
+      <c r="K148" s="5">
         <v>65</v>
       </c>
       <c r="L148">
@@ -12412,7 +12414,7 @@
       <c r="J149">
         <v>2</v>
       </c>
-      <c r="K149">
+      <c r="K149" s="5">
         <v>72</v>
       </c>
       <c r="L149">
@@ -12489,7 +12491,7 @@
       <c r="J150">
         <v>2</v>
       </c>
-      <c r="K150">
+      <c r="K150" s="5">
         <v>21</v>
       </c>
       <c r="L150">
@@ -12566,7 +12568,7 @@
       <c r="J151">
         <v>2</v>
       </c>
-      <c r="K151">
+      <c r="K151" s="5">
         <v>79</v>
       </c>
       <c r="L151">
@@ -12643,7 +12645,7 @@
       <c r="J152">
         <v>2</v>
       </c>
-      <c r="K152">
+      <c r="K152" s="5">
         <v>72</v>
       </c>
       <c r="L152">
@@ -12720,7 +12722,7 @@
       <c r="J153">
         <v>2</v>
       </c>
-      <c r="K153">
+      <c r="K153" s="5">
         <v>50</v>
       </c>
       <c r="L153">
@@ -12797,7 +12799,7 @@
       <c r="J154">
         <v>2</v>
       </c>
-      <c r="K154">
+      <c r="K154" s="5">
         <v>90</v>
       </c>
       <c r="L154">
@@ -12874,7 +12876,7 @@
       <c r="J155">
         <v>2</v>
       </c>
-      <c r="K155">
+      <c r="K155" s="5">
         <v>250</v>
       </c>
       <c r="L155">
@@ -12954,7 +12956,7 @@
       <c r="J156">
         <v>2</v>
       </c>
-      <c r="K156">
+      <c r="K156" s="5">
         <v>80</v>
       </c>
       <c r="L156">
@@ -13115,7 +13117,7 @@
       <c r="J157">
         <v>2</v>
       </c>
-      <c r="K157">
+      <c r="K157" s="5">
         <v>90</v>
       </c>
       <c r="L157">
@@ -13192,7 +13194,7 @@
       <c r="J158">
         <v>2</v>
       </c>
-      <c r="K158">
+      <c r="K158" s="5">
         <v>98</v>
       </c>
       <c r="L158">
@@ -13269,7 +13271,7 @@
       <c r="J159">
         <v>2</v>
       </c>
-      <c r="K159">
+      <c r="K159" s="5">
         <v>60</v>
       </c>
       <c r="L159">
@@ -13346,7 +13348,7 @@
       <c r="J160">
         <v>2</v>
       </c>
-      <c r="K160">
+      <c r="K160" s="5">
         <v>64</v>
       </c>
       <c r="L160">
@@ -13426,7 +13428,7 @@
       <c r="J161">
         <v>2</v>
       </c>
-      <c r="K161">
+      <c r="K161" s="5">
         <v>53</v>
       </c>
       <c r="L161">
@@ -13503,7 +13505,7 @@
       <c r="J162">
         <v>2</v>
       </c>
-      <c r="K162">
+      <c r="K162" s="5">
         <v>145</v>
       </c>
       <c r="L162">
@@ -13580,7 +13582,7 @@
       <c r="J163">
         <v>2</v>
       </c>
-      <c r="K163">
+      <c r="K163" s="5">
         <v>60</v>
       </c>
       <c r="L163">
@@ -13660,7 +13662,7 @@
       <c r="J164">
         <v>2</v>
       </c>
-      <c r="K164">
+      <c r="K164" s="5">
         <v>70</v>
       </c>
       <c r="L164">
@@ -13737,7 +13739,7 @@
       <c r="J165">
         <v>2</v>
       </c>
-      <c r="K165">
+      <c r="K165" s="5">
         <v>95</v>
       </c>
       <c r="L165">
@@ -13817,7 +13819,7 @@
       <c r="J166">
         <v>2</v>
       </c>
-      <c r="K166">
+      <c r="K166" s="5">
         <v>130</v>
       </c>
       <c r="L166">
@@ -13894,7 +13896,7 @@
       <c r="J167">
         <v>2</v>
       </c>
-      <c r="K167">
+      <c r="K167" s="5">
         <v>42</v>
       </c>
       <c r="L167">
@@ -13971,7 +13973,7 @@
       <c r="J168">
         <v>2</v>
       </c>
-      <c r="K168">
+      <c r="K168" s="5">
         <v>90</v>
       </c>
       <c r="L168">
@@ -14048,7 +14050,7 @@
       <c r="J169">
         <v>2</v>
       </c>
-      <c r="K169">
+      <c r="K169" s="5">
         <v>110</v>
       </c>
       <c r="L169">
@@ -14125,7 +14127,7 @@
       <c r="J170">
         <v>2</v>
       </c>
-      <c r="K170">
+      <c r="K170" s="5">
         <v>60</v>
       </c>
       <c r="L170">
@@ -14202,7 +14204,7 @@
       <c r="J171">
         <v>2</v>
       </c>
-      <c r="K171">
+      <c r="K171" s="5">
         <v>100</v>
       </c>
       <c r="L171">
@@ -14279,7 +14281,7 @@
       <c r="J172">
         <v>2</v>
       </c>
-      <c r="K172">
+      <c r="K172" s="5">
         <v>139</v>
       </c>
       <c r="L172">
@@ -14356,7 +14358,7 @@
       <c r="J173">
         <v>2</v>
       </c>
-      <c r="K173">
+      <c r="K173" s="5">
         <v>100</v>
       </c>
       <c r="L173">
@@ -14433,7 +14435,7 @@
       <c r="J174">
         <v>2</v>
       </c>
-      <c r="K174">
+      <c r="K174" s="5">
         <v>148</v>
       </c>
       <c r="L174">
@@ -14510,7 +14512,7 @@
       <c r="J175">
         <v>2</v>
       </c>
-      <c r="K175">
+      <c r="K175" s="5">
         <v>95</v>
       </c>
       <c r="L175">
@@ -14587,7 +14589,7 @@
       <c r="J176">
         <v>2</v>
       </c>
-      <c r="K176">
+      <c r="K176" s="5">
         <v>120</v>
       </c>
       <c r="L176">
@@ -14664,7 +14666,7 @@
       <c r="J177">
         <v>2</v>
       </c>
-      <c r="K177">
+      <c r="K177" s="5">
         <v>30</v>
       </c>
       <c r="L177">
@@ -14741,7 +14743,7 @@
       <c r="J178">
         <v>2</v>
       </c>
-      <c r="K178">
+      <c r="K178" s="5">
         <v>140</v>
       </c>
       <c r="L178">
@@ -14818,7 +14820,7 @@
       <c r="J179">
         <v>2</v>
       </c>
-      <c r="K179">
+      <c r="K179" s="5">
         <v>50</v>
       </c>
       <c r="L179">
@@ -14895,7 +14897,7 @@
       <c r="J180">
         <v>2</v>
       </c>
-      <c r="K180">
+      <c r="K180" s="5">
         <v>45</v>
       </c>
       <c r="L180">
@@ -14972,7 +14974,7 @@
       <c r="J181">
         <v>2</v>
       </c>
-      <c r="K181">
+      <c r="K181" s="5">
         <v>70</v>
       </c>
       <c r="L181">
@@ -15049,7 +15051,7 @@
       <c r="J182">
         <v>2</v>
       </c>
-      <c r="K182">
+      <c r="K182" s="5">
         <v>34</v>
       </c>
       <c r="L182">
@@ -15126,7 +15128,7 @@
       <c r="J183">
         <v>2</v>
       </c>
-      <c r="K183">
+      <c r="K183" s="5">
         <v>35</v>
       </c>
       <c r="L183">
@@ -15203,7 +15205,7 @@
       <c r="J184">
         <v>2</v>
       </c>
-      <c r="K184">
+      <c r="K184" s="5">
         <v>85</v>
       </c>
       <c r="L184">
@@ -15280,7 +15282,7 @@
       <c r="J185">
         <v>1</v>
       </c>
-      <c r="K185">
+      <c r="K185" s="5">
         <v>130</v>
       </c>
       <c r="L185">
@@ -15357,7 +15359,7 @@
       <c r="J186">
         <v>2</v>
       </c>
-      <c r="K186">
+      <c r="K186" s="5">
         <v>100</v>
       </c>
       <c r="L186">
@@ -15437,7 +15439,7 @@
       <c r="J187">
         <v>2</v>
       </c>
-      <c r="K187">
+      <c r="K187" s="5">
         <v>80</v>
       </c>
       <c r="L187">
@@ -15514,7 +15516,7 @@
       <c r="J188">
         <v>2</v>
       </c>
-      <c r="K188">
+      <c r="K188" s="5">
         <v>70</v>
       </c>
       <c r="L188">
@@ -15591,7 +15593,7 @@
       <c r="J189">
         <v>2</v>
       </c>
-      <c r="K189">
+      <c r="K189" s="5">
         <v>95</v>
       </c>
       <c r="L189">
@@ -15668,7 +15670,7 @@
       <c r="J190">
         <v>2</v>
       </c>
-      <c r="K190">
+      <c r="K190" s="5">
         <v>60</v>
       </c>
       <c r="L190">
@@ -15745,7 +15747,7 @@
       <c r="J191">
         <v>2</v>
       </c>
-      <c r="K191">
+      <c r="K191" s="5">
         <v>15</v>
       </c>
       <c r="L191">
@@ -15822,7 +15824,7 @@
       <c r="J192">
         <v>2</v>
       </c>
-      <c r="K192">
+      <c r="K192" s="5">
         <v>134</v>
       </c>
       <c r="L192">
@@ -15899,7 +15901,7 @@
       <c r="J193">
         <v>2</v>
       </c>
-      <c r="K193">
+      <c r="K193" s="5">
         <v>45</v>
       </c>
       <c r="L193">
@@ -15976,7 +15978,7 @@
       <c r="J194">
         <v>2</v>
       </c>
-      <c r="K194">
+      <c r="K194" s="5">
         <v>84</v>
       </c>
       <c r="L194">
@@ -16053,7 +16055,7 @@
       <c r="J195">
         <v>2</v>
       </c>
-      <c r="K195">
+      <c r="K195" s="5">
         <v>30</v>
       </c>
       <c r="L195">
@@ -16130,7 +16132,7 @@
       <c r="J196">
         <v>2</v>
       </c>
-      <c r="K196">
+      <c r="K196" s="5">
         <v>73</v>
       </c>
       <c r="L196">
@@ -16207,7 +16209,7 @@
       <c r="J197">
         <v>2</v>
       </c>
-      <c r="K197">
+      <c r="K197" s="5">
         <v>80</v>
       </c>
       <c r="L197">
@@ -16284,7 +16286,7 @@
       <c r="J198">
         <v>2</v>
       </c>
-      <c r="K198">
+      <c r="K198" s="5">
         <v>50</v>
       </c>
       <c r="L198">
@@ -16361,7 +16363,7 @@
       <c r="J199">
         <v>2</v>
       </c>
-      <c r="K199">
+      <c r="K199" s="5">
         <v>50</v>
       </c>
       <c r="L199">
@@ -16438,7 +16440,7 @@
       <c r="J200">
         <v>2</v>
       </c>
-      <c r="K200">
+      <c r="K200" s="5">
         <v>127</v>
       </c>
       <c r="L200">
@@ -16515,7 +16517,7 @@
       <c r="J201">
         <v>2</v>
       </c>
-      <c r="K201">
+      <c r="K201" s="5">
         <v>20</v>
       </c>
       <c r="L201">
@@ -16592,7 +16594,7 @@
       <c r="J202">
         <v>2</v>
       </c>
-      <c r="K202">
+      <c r="K202" s="5">
         <v>40</v>
       </c>
       <c r="L202">
@@ -16669,7 +16671,7 @@
       <c r="J203">
         <v>2</v>
       </c>
-      <c r="K203">
+      <c r="K203" s="5">
         <v>105</v>
       </c>
       <c r="L203">
@@ -16746,7 +16748,7 @@
       <c r="J204">
         <v>2</v>
       </c>
-      <c r="K204">
+      <c r="K204" s="5">
         <v>45</v>
       </c>
       <c r="L204">
@@ -16823,7 +16825,7 @@
       <c r="J205">
         <v>2</v>
       </c>
-      <c r="K205">
+      <c r="K205" s="5">
         <v>70</v>
       </c>
       <c r="L205">
@@ -16900,7 +16902,7 @@
       <c r="J206">
         <v>2</v>
       </c>
-      <c r="K206">
+      <c r="K206" s="5">
         <v>100</v>
       </c>
       <c r="L206">
@@ -16977,7 +16979,7 @@
       <c r="J207">
         <v>2</v>
       </c>
-      <c r="K207">
+      <c r="K207" s="5">
         <v>85</v>
       </c>
       <c r="L207">
@@ -17054,7 +17056,7 @@
       <c r="J208">
         <v>2</v>
       </c>
-      <c r="K208">
+      <c r="K208" s="5">
         <v>50</v>
       </c>
       <c r="L208">
@@ -17131,7 +17133,7 @@
       <c r="J209">
         <v>2</v>
       </c>
-      <c r="K209">
+      <c r="K209" s="5">
         <v>70</v>
       </c>
       <c r="L209">
@@ -17208,7 +17210,7 @@
       <c r="J210">
         <v>2</v>
       </c>
-      <c r="K210">
+      <c r="K210" s="5">
         <v>43</v>
       </c>
       <c r="L210">
@@ -17285,7 +17287,7 @@
       <c r="J211">
         <v>2</v>
       </c>
-      <c r="K211">
+      <c r="K211" s="5">
         <v>35</v>
       </c>
       <c r="L211">
@@ -17362,7 +17364,7 @@
       <c r="J212">
         <v>2</v>
       </c>
-      <c r="K212">
+      <c r="K212" s="5">
         <v>28</v>
       </c>
       <c r="L212">
@@ -17439,7 +17441,7 @@
       <c r="J213">
         <v>2</v>
       </c>
-      <c r="K213">
+      <c r="K213" s="5">
         <v>45</v>
       </c>
       <c r="L213">
@@ -17516,7 +17518,7 @@
       <c r="J214">
         <v>2</v>
       </c>
-      <c r="K214">
+      <c r="K214" s="5">
         <v>100</v>
       </c>
       <c r="L214">
@@ -17593,7 +17595,7 @@
       <c r="J215">
         <v>2</v>
       </c>
-      <c r="K215">
+      <c r="K215" s="5">
         <v>86</v>
       </c>
       <c r="L215">
@@ -17670,7 +17672,7 @@
       <c r="J216">
         <v>2</v>
       </c>
-      <c r="K216">
+      <c r="K216" s="5">
         <v>92</v>
       </c>
       <c r="L216">
@@ -17747,7 +17749,7 @@
       <c r="J217">
         <v>2</v>
       </c>
-      <c r="K217">
+      <c r="K217" s="5">
         <v>90</v>
       </c>
       <c r="L217">
@@ -17824,7 +17826,7 @@
       <c r="J218">
         <v>2</v>
       </c>
-      <c r="K218">
+      <c r="K218" s="5">
         <v>95</v>
       </c>
       <c r="L218">
@@ -17901,7 +17903,7 @@
       <c r="J219">
         <v>2</v>
       </c>
-      <c r="K219">
+      <c r="K219" s="5">
         <v>30</v>
       </c>
       <c r="L219">
@@ -17978,7 +17980,7 @@
       <c r="J220">
         <v>2</v>
       </c>
-      <c r="K220">
+      <c r="K220" s="5">
         <v>135</v>
       </c>
       <c r="L220">
@@ -18055,7 +18057,7 @@
       <c r="J221">
         <v>2</v>
       </c>
-      <c r="K221">
+      <c r="K221" s="5">
         <v>85</v>
       </c>
       <c r="L221">
@@ -18132,7 +18134,7 @@
       <c r="J222">
         <v>2</v>
       </c>
-      <c r="K222">
+      <c r="K222" s="5">
         <v>75</v>
       </c>
       <c r="L222">
@@ -18209,7 +18211,7 @@
       <c r="J223">
         <v>2</v>
       </c>
-      <c r="K223">
+      <c r="K223" s="5">
         <v>60</v>
       </c>
       <c r="L223">
@@ -18286,7 +18288,7 @@
       <c r="J224">
         <v>2</v>
       </c>
-      <c r="K224">
+      <c r="K224" s="5">
         <v>55</v>
       </c>
       <c r="L224">
@@ -18363,7 +18365,7 @@
       <c r="J225">
         <v>1</v>
       </c>
-      <c r="K225">
+      <c r="K225" s="5">
         <v>40</v>
       </c>
       <c r="L225">
@@ -18440,7 +18442,7 @@
       <c r="J226">
         <v>2</v>
       </c>
-      <c r="K226">
+      <c r="K226" s="5">
         <v>64</v>
       </c>
       <c r="L226">
@@ -18517,7 +18519,7 @@
       <c r="J227">
         <v>2</v>
       </c>
-      <c r="K227">
+      <c r="K227" s="5">
         <v>75</v>
       </c>
       <c r="L227">
@@ -18594,7 +18596,7 @@
       <c r="J228">
         <v>0.5</v>
       </c>
-      <c r="K228">
+      <c r="K228" s="5">
         <v>110</v>
       </c>
       <c r="L228">
@@ -18671,7 +18673,7 @@
       <c r="J229">
         <v>2</v>
       </c>
-      <c r="K229">
+      <c r="K229" s="5">
         <v>64</v>
       </c>
       <c r="L229">
@@ -18748,7 +18750,7 @@
       <c r="J230">
         <v>2</v>
       </c>
-      <c r="K230">
+      <c r="K230" s="5">
         <v>80</v>
       </c>
       <c r="L230">
@@ -18825,7 +18827,7 @@
       <c r="J231">
         <v>2</v>
       </c>
-      <c r="K231">
+      <c r="K231" s="5">
         <v>20</v>
       </c>
       <c r="L231">
@@ -18902,7 +18904,7 @@
       <c r="J232">
         <v>2</v>
       </c>
-      <c r="K232">
+      <c r="K232" s="5">
         <v>90</v>
       </c>
       <c r="L232">
@@ -18979,7 +18981,7 @@
       <c r="J233">
         <v>2</v>
       </c>
-      <c r="K233">
+      <c r="K233" s="5">
         <v>95</v>
       </c>
       <c r="L233">
@@ -19056,7 +19058,7 @@
       <c r="J234">
         <v>2</v>
       </c>
-      <c r="K234">
+      <c r="K234" s="5">
         <v>75</v>
       </c>
       <c r="L234">
@@ -19133,7 +19135,7 @@
       <c r="J235">
         <v>2</v>
       </c>
-      <c r="K235">
+      <c r="K235" s="5">
         <v>150</v>
       </c>
       <c r="L235">
@@ -19213,7 +19215,7 @@
       <c r="J236">
         <v>2</v>
       </c>
-      <c r="K236">
+      <c r="K236" s="5">
         <v>100</v>
       </c>
       <c r="L236">
@@ -19293,7 +19295,7 @@
       <c r="J237">
         <v>2</v>
       </c>
-      <c r="K237">
+      <c r="K237" s="5">
         <v>70</v>
       </c>
       <c r="L237">
@@ -19370,7 +19372,7 @@
       <c r="J238">
         <v>2</v>
       </c>
-      <c r="K238">
+      <c r="K238" s="5">
         <v>90</v>
       </c>
       <c r="L238">
@@ -19444,7 +19446,7 @@
       <c r="J239">
         <v>2</v>
       </c>
-      <c r="K239">
+      <c r="K239" s="5">
         <v>100</v>
       </c>
       <c r="L239">
@@ -19521,7 +19523,7 @@
       <c r="J240">
         <v>2</v>
       </c>
-      <c r="K240">
+      <c r="K240" s="5">
         <v>70</v>
       </c>
       <c r="L240">
@@ -19598,7 +19600,7 @@
       <c r="J241">
         <v>2</v>
       </c>
-      <c r="K241">
+      <c r="K241" s="5">
         <v>100</v>
       </c>
       <c r="L241">
@@ -19675,7 +19677,7 @@
       <c r="J242">
         <v>2</v>
       </c>
-      <c r="K242">
+      <c r="K242" s="5">
         <v>65</v>
       </c>
       <c r="L242">
@@ -19752,7 +19754,7 @@
       <c r="J243">
         <v>2</v>
       </c>
-      <c r="K243">
+      <c r="K243" s="5">
         <v>65</v>
       </c>
       <c r="L243">
@@ -19829,7 +19831,7 @@
       <c r="J244">
         <v>2</v>
       </c>
-      <c r="K244">
+      <c r="K244" s="5">
         <v>80</v>
       </c>
       <c r="L244">
@@ -19906,7 +19908,7 @@
       <c r="J245">
         <v>2</v>
       </c>
-      <c r="K245">
+      <c r="K245" s="5">
         <v>100</v>
       </c>
       <c r="L245">
@@ -19983,7 +19985,7 @@
       <c r="J246">
         <v>2</v>
       </c>
-      <c r="K246">
+      <c r="K246" s="5">
         <v>10</v>
       </c>
       <c r="L246">
@@ -20060,7 +20062,7 @@
       <c r="J247">
         <v>2</v>
       </c>
-      <c r="K247">
+      <c r="K247" s="5">
         <v>10</v>
       </c>
       <c r="L247">
@@ -20137,7 +20139,7 @@
       <c r="J248">
         <v>2</v>
       </c>
-      <c r="K248">
+      <c r="K248" s="5">
         <v>25</v>
       </c>
       <c r="L248">
@@ -20214,7 +20216,7 @@
       <c r="J249">
         <v>2</v>
       </c>
-      <c r="K249">
+      <c r="K249" s="5">
         <v>60</v>
       </c>
       <c r="L249">
@@ -20291,7 +20293,7 @@
       <c r="J250">
         <v>2</v>
       </c>
-      <c r="K250">
+      <c r="K250" s="5">
         <v>45</v>
       </c>
       <c r="L250">
@@ -20368,7 +20370,7 @@
       <c r="J251">
         <v>2</v>
       </c>
-      <c r="K251">
+      <c r="K251" s="5">
         <v>42</v>
       </c>
       <c r="L251">
@@ -20445,7 +20447,7 @@
       <c r="J252">
         <v>2</v>
       </c>
-      <c r="K252">
+      <c r="K252" s="5">
         <v>150</v>
       </c>
       <c r="L252">
@@ -20522,7 +20524,7 @@
       <c r="J253">
         <v>2</v>
       </c>
-      <c r="K253">
+      <c r="K253" s="5">
         <v>46</v>
       </c>
       <c r="L253">
@@ -20599,7 +20601,7 @@
       <c r="J254">
         <v>2</v>
       </c>
-      <c r="K254">
+      <c r="K254" s="5">
         <v>75</v>
       </c>
       <c r="L254">
@@ -20676,7 +20678,7 @@
       <c r="J255">
         <v>2</v>
       </c>
-      <c r="K255">
+      <c r="K255" s="5">
         <v>195</v>
       </c>
       <c r="L255">
@@ -20753,7 +20755,7 @@
       <c r="J256">
         <v>2</v>
       </c>
-      <c r="K256">
+      <c r="K256" s="5">
         <v>170</v>
       </c>
       <c r="L256">
@@ -20833,7 +20835,7 @@
       <c r="J257">
         <v>2</v>
       </c>
-      <c r="K257">
+      <c r="K257" s="5">
         <v>59</v>
       </c>
       <c r="L257">
@@ -20910,7 +20912,7 @@
       <c r="J258">
         <v>2</v>
       </c>
-      <c r="K258">
+      <c r="K258" s="5">
         <v>80</v>
       </c>
       <c r="L258">
@@ -20987,7 +20989,7 @@
       <c r="J259">
         <v>2</v>
       </c>
-      <c r="K259">
+      <c r="K259" s="5">
         <v>66</v>
       </c>
       <c r="L259">
@@ -21064,7 +21066,7 @@
       <c r="J260">
         <v>2</v>
       </c>
-      <c r="K260">
+      <c r="K260" s="5">
         <v>115</v>
       </c>
       <c r="L260">
@@ -21141,7 +21143,7 @@
       <c r="J261">
         <v>2</v>
       </c>
-      <c r="K261">
+      <c r="K261" s="5">
         <v>120</v>
       </c>
       <c r="L261">
@@ -21218,7 +21220,7 @@
       <c r="J262">
         <v>2</v>
       </c>
-      <c r="K262">
+      <c r="K262" s="5">
         <v>100</v>
       </c>
       <c r="L262">
@@ -21295,7 +21297,7 @@
       <c r="J263">
         <v>2</v>
       </c>
-      <c r="K263">
+      <c r="K263" s="5">
         <v>57</v>
       </c>
       <c r="L263">
@@ -21372,7 +21374,7 @@
       <c r="J264">
         <v>2</v>
       </c>
-      <c r="K264">
+      <c r="K264" s="5">
         <v>65</v>
       </c>
       <c r="L264">
@@ -21449,7 +21451,7 @@
       <c r="J265">
         <v>2</v>
       </c>
-      <c r="K265">
+      <c r="K265" s="5">
         <v>57</v>
       </c>
       <c r="L265">
@@ -21526,7 +21528,7 @@
       <c r="J266">
         <v>2</v>
       </c>
-      <c r="K266">
+      <c r="K266" s="5">
         <v>65</v>
       </c>
       <c r="L266">
@@ -21603,7 +21605,7 @@
       <c r="J267">
         <v>2</v>
       </c>
-      <c r="K267">
+      <c r="K267" s="5">
         <v>60</v>
       </c>
       <c r="L267">
@@ -21680,7 +21682,7 @@
       <c r="J268">
         <v>2</v>
       </c>
-      <c r="K268">
+      <c r="K268" s="5">
         <v>78</v>
       </c>
       <c r="L268">
@@ -21757,7 +21759,7 @@
       <c r="J269">
         <v>2</v>
       </c>
-      <c r="K269">
+      <c r="K269" s="5">
         <v>119</v>
       </c>
       <c r="L269">
@@ -21834,7 +21836,7 @@
       <c r="J270">
         <v>2</v>
       </c>
-      <c r="K270">
+      <c r="K270" s="5">
         <v>50</v>
       </c>
       <c r="L270">
@@ -21911,7 +21913,7 @@
       <c r="J271">
         <v>2</v>
       </c>
-      <c r="K271">
+      <c r="K271" s="5">
         <v>92</v>
       </c>
       <c r="L271">
@@ -21988,7 +21990,7 @@
       <c r="J272">
         <v>2</v>
       </c>
-      <c r="K272">
+      <c r="K272" s="5">
         <v>55</v>
       </c>
       <c r="L272">
@@ -22065,7 +22067,7 @@
       <c r="J273">
         <v>2</v>
       </c>
-      <c r="K273">
+      <c r="K273" s="5">
         <v>45</v>
       </c>
       <c r="L273">
@@ -22142,7 +22144,7 @@
       <c r="J274">
         <v>2</v>
       </c>
-      <c r="K274">
+      <c r="K274" s="5">
         <v>35</v>
       </c>
       <c r="L274">
@@ -22219,7 +22221,7 @@
       <c r="J275">
         <v>2</v>
       </c>
-      <c r="K275">
+      <c r="K275" s="5">
         <v>130</v>
       </c>
       <c r="L275">
@@ -22296,7 +22298,7 @@
       <c r="J276">
         <v>2</v>
       </c>
-      <c r="K276">
+      <c r="K276" s="5">
         <v>28</v>
       </c>
       <c r="L276">
@@ -22373,7 +22375,7 @@
       <c r="J277">
         <v>2</v>
       </c>
-      <c r="K277">
+      <c r="K277" s="5">
         <v>90</v>
       </c>
       <c r="L277">
@@ -22450,7 +22452,7 @@
       <c r="J278">
         <v>2</v>
       </c>
-      <c r="K278">
+      <c r="K278" s="5">
         <v>40</v>
       </c>
       <c r="L278">
@@ -22527,7 +22529,7 @@
       <c r="J279">
         <v>2</v>
       </c>
-      <c r="K279">
+      <c r="K279" s="5">
         <v>130</v>
       </c>
       <c r="L279">
@@ -22604,7 +22606,7 @@
       <c r="J280">
         <v>2</v>
       </c>
-      <c r="K280">
+      <c r="K280" s="5">
         <v>65</v>
       </c>
       <c r="L280">
@@ -22681,7 +22683,7 @@
       <c r="J281">
         <v>2</v>
       </c>
-      <c r="K281">
+      <c r="K281" s="5">
         <v>35</v>
       </c>
       <c r="L281">
@@ -22758,7 +22760,7 @@
       <c r="J282">
         <v>2</v>
       </c>
-      <c r="K282">
+      <c r="K282" s="5">
         <v>50</v>
       </c>
       <c r="L282">
@@ -22835,7 +22837,7 @@
       <c r="J283">
         <v>2</v>
       </c>
-      <c r="K283">
+      <c r="K283" s="5">
         <v>50</v>
       </c>
       <c r="L283">
@@ -22912,7 +22914,7 @@
       <c r="J284">
         <v>2</v>
       </c>
-      <c r="K284">
+      <c r="K284" s="5">
         <v>90</v>
       </c>
       <c r="L284">
@@ -22989,7 +22991,7 @@
       <c r="J285">
         <v>1</v>
       </c>
-      <c r="K285">
+      <c r="K285" s="5">
         <v>32</v>
       </c>
       <c r="L285">
@@ -23066,7 +23068,7 @@
       <c r="J286">
         <v>2</v>
       </c>
-      <c r="K286">
+      <c r="K286" s="5">
         <v>60</v>
       </c>
       <c r="L286">
@@ -23143,7 +23145,7 @@
       <c r="J287">
         <v>2</v>
       </c>
-      <c r="K287">
+      <c r="K287" s="5">
         <v>85</v>
       </c>
       <c r="L287">
@@ -23220,7 +23222,7 @@
       <c r="J288">
         <v>2</v>
       </c>
-      <c r="K288">
+      <c r="K288" s="5">
         <v>41</v>
       </c>
       <c r="L288">
@@ -23297,7 +23299,7 @@
       <c r="J289">
         <v>2</v>
       </c>
-      <c r="K289">
+      <c r="K289" s="5">
         <v>52</v>
       </c>
       <c r="L289">
@@ -23374,7 +23376,7 @@
       <c r="J290">
         <v>2</v>
       </c>
-      <c r="K290">
+      <c r="K290" s="5">
         <v>50</v>
       </c>
       <c r="L290">
@@ -23451,7 +23453,7 @@
       <c r="J291">
         <v>2</v>
       </c>
-      <c r="K291">
+      <c r="K291" s="5">
         <v>99</v>
       </c>
       <c r="L291">
@@ -23528,7 +23530,7 @@
       <c r="J292">
         <v>2</v>
       </c>
-      <c r="K292">
+      <c r="K292" s="5">
         <v>33</v>
       </c>
       <c r="L292">
@@ -23605,7 +23607,7 @@
       <c r="J293">
         <v>2</v>
       </c>
-      <c r="K293">
+      <c r="K293" s="5">
         <v>127</v>
       </c>
       <c r="L293">
@@ -23682,7 +23684,7 @@
       <c r="J294">
         <v>2</v>
       </c>
-      <c r="K294">
+      <c r="K294" s="5">
         <v>145</v>
       </c>
       <c r="L294">
@@ -23759,7 +23761,7 @@
       <c r="J295">
         <v>2</v>
       </c>
-      <c r="K295">
+      <c r="K295" s="5">
         <v>100</v>
       </c>
       <c r="L295">
@@ -23836,7 +23838,7 @@
       <c r="J296">
         <v>2</v>
       </c>
-      <c r="K296">
+      <c r="K296" s="5">
         <v>40</v>
       </c>
       <c r="L296">
@@ -23913,7 +23915,7 @@
       <c r="J297">
         <v>2</v>
       </c>
-      <c r="K297">
+      <c r="K297" s="5">
         <v>95</v>
       </c>
       <c r="L297">
@@ -23990,7 +23992,7 @@
       <c r="J298">
         <v>2</v>
       </c>
-      <c r="K298">
+      <c r="K298" s="5">
         <v>65</v>
       </c>
       <c r="L298">
@@ -24067,7 +24069,7 @@
       <c r="J299">
         <v>2</v>
       </c>
-      <c r="K299">
+      <c r="K299" s="5">
         <v>55</v>
       </c>
       <c r="L299">
@@ -24144,7 +24146,7 @@
       <c r="J300">
         <v>2</v>
       </c>
-      <c r="K300">
+      <c r="K300" s="5">
         <v>150</v>
       </c>
       <c r="L300">
@@ -24224,7 +24226,7 @@
       <c r="J301">
         <v>2</v>
       </c>
-      <c r="K301">
+      <c r="K301" s="5">
         <v>85</v>
       </c>
       <c r="L301">
@@ -24301,7 +24303,7 @@
       <c r="J302">
         <v>2</v>
       </c>
-      <c r="K302">
+      <c r="K302" s="5">
         <v>125</v>
       </c>
       <c r="L302">
@@ -24378,7 +24380,7 @@
       <c r="J303">
         <v>2</v>
       </c>
-      <c r="K303">
+      <c r="K303" s="5">
         <v>40</v>
       </c>
       <c r="L303">
@@ -24455,7 +24457,7 @@
       <c r="J304">
         <v>2</v>
       </c>
-      <c r="K304">
+      <c r="K304" s="5">
         <v>70</v>
       </c>
       <c r="L304">
@@ -24532,7 +24534,7 @@
       <c r="J305">
         <v>2</v>
       </c>
-      <c r="K305">
+      <c r="K305" s="5">
         <v>54</v>
       </c>
       <c r="L305">
@@ -24609,7 +24611,7 @@
       <c r="J306">
         <v>2</v>
       </c>
-      <c r="K306">
+      <c r="K306" s="5">
         <v>60</v>
       </c>
       <c r="L306">
@@ -24686,7 +24688,7 @@
       <c r="J307">
         <v>2</v>
       </c>
-      <c r="K307">
+      <c r="K307" s="5">
         <v>120</v>
       </c>
       <c r="L307">
@@ -24760,7 +24762,7 @@
       <c r="I308" t="s">
         <v>30</v>
       </c>
-      <c r="K308">
+      <c r="K308" s="5">
         <v>25</v>
       </c>
       <c r="L308">
@@ -24831,7 +24833,7 @@
       <c r="I309" t="s">
         <v>30</v>
       </c>
-      <c r="K309">
+      <c r="K309" s="5">
         <v>100</v>
       </c>
       <c r="L309">
@@ -24902,7 +24904,7 @@
       <c r="I310" t="s">
         <v>30</v>
       </c>
-      <c r="K310">
+      <c r="K310" s="5">
         <v>95</v>
       </c>
       <c r="L310">
@@ -24973,7 +24975,7 @@
       <c r="I311" t="s">
         <v>30</v>
       </c>
-      <c r="K311">
+      <c r="K311" s="5">
         <v>55</v>
       </c>
       <c r="L311">
@@ -25044,7 +25046,7 @@
       <c r="I312" t="s">
         <v>30</v>
       </c>
-      <c r="K312">
+      <c r="K312" s="5">
         <v>40</v>
       </c>
       <c r="L312">
@@ -25115,7 +25117,7 @@
       <c r="I313" t="s">
         <v>30</v>
       </c>
-      <c r="K313">
+      <c r="K313" s="5">
         <v>140</v>
       </c>
       <c r="L313">
@@ -25186,7 +25188,7 @@
       <c r="I314" t="s">
         <v>30</v>
       </c>
-      <c r="K314">
+      <c r="K314" s="5">
         <v>50</v>
       </c>
       <c r="L314">
@@ -25257,7 +25259,7 @@
       <c r="I315" t="s">
         <v>30</v>
       </c>
-      <c r="K315">
+      <c r="K315" s="5">
         <v>65</v>
       </c>
       <c r="L315">
@@ -25328,7 +25330,7 @@
       <c r="I316" t="s">
         <v>30</v>
       </c>
-      <c r="K316">
+      <c r="K316" s="5">
         <v>45</v>
       </c>
       <c r="L316">
@@ -25399,7 +25401,7 @@
       <c r="I317" t="s">
         <v>30</v>
       </c>
-      <c r="K317">
+      <c r="K317" s="5">
         <v>70</v>
       </c>
       <c r="L317">
@@ -25470,7 +25472,7 @@
       <c r="I318" t="s">
         <v>30</v>
       </c>
-      <c r="K318">
+      <c r="K318" s="5">
         <v>60</v>
       </c>
       <c r="L318">
@@ -25544,7 +25546,7 @@
       <c r="I319" t="s">
         <v>30</v>
       </c>
-      <c r="K319">
+      <c r="K319" s="5">
         <v>80</v>
       </c>
       <c r="L319">
@@ -25615,7 +25617,7 @@
       <c r="I320" t="s">
         <v>30</v>
       </c>
-      <c r="K320">
+      <c r="K320" s="5">
         <v>90</v>
       </c>
       <c r="L320">
@@ -25686,7 +25688,7 @@
       <c r="I321" t="s">
         <v>30</v>
       </c>
-      <c r="K321">
+      <c r="K321" s="5">
         <v>62</v>
       </c>
       <c r="L321">
@@ -25757,7 +25759,7 @@
       <c r="I322" t="s">
         <v>30</v>
       </c>
-      <c r="K322">
+      <c r="K322" s="5">
         <v>37</v>
       </c>
       <c r="L322">
@@ -25828,7 +25830,7 @@
       <c r="I323" t="s">
         <v>30</v>
       </c>
-      <c r="K323">
+      <c r="K323" s="5">
         <v>150</v>
       </c>
       <c r="L323">
@@ -25899,7 +25901,7 @@
       <c r="I324" t="s">
         <v>30</v>
       </c>
-      <c r="K324">
+      <c r="K324" s="5">
         <v>75</v>
       </c>
       <c r="L324">
@@ -25970,7 +25972,7 @@
       <c r="I325" t="s">
         <v>30</v>
       </c>
-      <c r="K325">
+      <c r="K325" s="5">
         <v>35</v>
       </c>
       <c r="L325">
@@ -26041,7 +26043,7 @@
       <c r="I326" t="s">
         <v>30</v>
       </c>
-      <c r="K326">
+      <c r="K326" s="5">
         <v>125</v>
       </c>
       <c r="L326">
@@ -26112,7 +26114,7 @@
       <c r="I327" t="s">
         <v>30</v>
       </c>
-      <c r="K327">
+      <c r="K327" s="5">
         <v>20</v>
       </c>
       <c r="L327">
@@ -26183,7 +26185,7 @@
       <c r="I328" t="s">
         <v>30</v>
       </c>
-      <c r="K328">
+      <c r="K328" s="5">
         <v>30</v>
       </c>
       <c r="L328">
@@ -26254,7 +26256,7 @@
       <c r="I329" t="s">
         <v>30</v>
       </c>
-      <c r="K329">
+      <c r="K329" s="5">
         <v>131</v>
       </c>
       <c r="L329">
@@ -26325,7 +26327,7 @@
       <c r="I330" t="s">
         <v>30</v>
       </c>
-      <c r="K330">
+      <c r="K330" s="5">
         <v>115</v>
       </c>
       <c r="L330">
@@ -26396,7 +26398,7 @@
       <c r="I331" t="s">
         <v>30</v>
       </c>
-      <c r="K331">
+      <c r="K331" s="5">
         <v>150</v>
       </c>
       <c r="L331">
@@ -26467,7 +26469,7 @@
       <c r="I332" t="s">
         <v>30</v>
       </c>
-      <c r="K332">
+      <c r="K332" s="5">
         <v>146</v>
       </c>
       <c r="L332">
@@ -26538,7 +26540,7 @@
       <c r="I333" t="s">
         <v>30</v>
       </c>
-      <c r="K333">
+      <c r="K333" s="5">
         <v>150</v>
       </c>
       <c r="L333">
@@ -26609,7 +26611,7 @@
       <c r="I334" t="s">
         <v>30</v>
       </c>
-      <c r="K334">
+      <c r="K334" s="5">
         <v>50</v>
       </c>
       <c r="L334">
@@ -26680,7 +26682,7 @@
       <c r="I335" t="s">
         <v>30</v>
       </c>
-      <c r="K335">
+      <c r="K335" s="5">
         <v>50</v>
       </c>
       <c r="L335">
@@ -26751,7 +26753,7 @@
       <c r="I336" t="s">
         <v>30</v>
       </c>
-      <c r="K336">
+      <c r="K336" s="5">
         <v>80</v>
       </c>
       <c r="L336">
@@ -26822,7 +26824,7 @@
       <c r="I337" t="s">
         <v>30</v>
       </c>
-      <c r="K337">
+      <c r="K337" s="5">
         <v>42</v>
       </c>
       <c r="L337">
@@ -26893,7 +26895,7 @@
       <c r="I338" t="s">
         <v>30</v>
       </c>
-      <c r="K338">
+      <c r="K338" s="5">
         <v>40</v>
       </c>
       <c r="L338">
@@ -26964,7 +26966,7 @@
       <c r="I339" t="s">
         <v>30</v>
       </c>
-      <c r="K339">
+      <c r="K339" s="5">
         <v>65</v>
       </c>
       <c r="L339">
@@ -27035,7 +27037,7 @@
       <c r="I340" t="s">
         <v>30</v>
       </c>
-      <c r="K340">
+      <c r="K340" s="5">
         <v>65</v>
       </c>
       <c r="L340">
@@ -27106,7 +27108,7 @@
       <c r="I341" t="s">
         <v>30</v>
       </c>
-      <c r="K341">
+      <c r="K341" s="5">
         <v>65</v>
       </c>
       <c r="L341">
@@ -27177,7 +27179,7 @@
       <c r="I342" t="s">
         <v>30</v>
       </c>
-      <c r="K342">
+      <c r="K342" s="5">
         <v>74</v>
       </c>
       <c r="L342">
@@ -27254,7 +27256,7 @@
       <c r="I343" t="s">
         <v>30</v>
       </c>
-      <c r="K343">
+      <c r="K343" s="5">
         <v>138</v>
       </c>
       <c r="L343">
@@ -27331,7 +27333,7 @@
       <c r="I344" t="s">
         <v>30</v>
       </c>
-      <c r="K344">
+      <c r="K344" s="5">
         <v>101</v>
       </c>
       <c r="L344">
@@ -27405,7 +27407,7 @@
       <c r="I345" t="s">
         <v>30</v>
       </c>
-      <c r="K345">
+      <c r="K345" s="5">
         <v>59</v>
       </c>
       <c r="L345">
@@ -27482,7 +27484,7 @@
       <c r="I346" t="s">
         <v>30</v>
       </c>
-      <c r="K346">
+      <c r="K346" s="5">
         <v>47</v>
       </c>
       <c r="L346">
@@ -27559,7 +27561,7 @@
       <c r="I347" t="s">
         <v>30</v>
       </c>
-      <c r="K347">
+      <c r="K347" s="5">
         <v>47</v>
       </c>
       <c r="L347">
@@ -27636,7 +27638,7 @@
       <c r="I348" t="s">
         <v>30</v>
       </c>
-      <c r="K348">
+      <c r="K348" s="5">
         <v>288</v>
       </c>
       <c r="L348">
@@ -27710,7 +27712,7 @@
       <c r="I349" t="s">
         <v>30</v>
       </c>
-      <c r="K349">
+      <c r="K349" s="5">
         <v>290</v>
       </c>
       <c r="L349">
@@ -27787,7 +27789,7 @@
       <c r="I350" t="s">
         <v>30</v>
       </c>
-      <c r="K350">
+      <c r="K350" s="5">
         <v>82</v>
       </c>
       <c r="L350">
@@ -27864,7 +27866,7 @@
       <c r="I351" t="s">
         <v>30</v>
       </c>
-      <c r="K351">
+      <c r="K351" s="5">
         <v>60</v>
       </c>
       <c r="L351">
@@ -27941,7 +27943,7 @@
       <c r="I352" t="s">
         <v>30</v>
       </c>
-      <c r="K352">
+      <c r="K352" s="5">
         <v>125</v>
       </c>
       <c r="L352">
@@ -28018,7 +28020,7 @@
       <c r="I353" t="s">
         <v>30</v>
       </c>
-      <c r="K353">
+      <c r="K353" s="5">
         <v>138</v>
       </c>
       <c r="L353">
@@ -28095,7 +28097,7 @@
       <c r="I354" t="s">
         <v>30</v>
       </c>
-      <c r="K354">
+      <c r="K354" s="5">
         <v>100</v>
       </c>
       <c r="L354">
@@ -28166,7 +28168,7 @@
       <c r="I355" t="s">
         <v>30</v>
       </c>
-      <c r="K355">
+      <c r="K355" s="5">
         <v>25</v>
       </c>
       <c r="L355">
@@ -28243,7 +28245,7 @@
       <c r="I356" t="s">
         <v>30</v>
       </c>
-      <c r="K356">
+      <c r="K356" s="5">
         <v>150</v>
       </c>
       <c r="L356">
@@ -28320,7 +28322,7 @@
       <c r="I357" t="s">
         <v>30</v>
       </c>
-      <c r="K357">
+      <c r="K357" s="5">
         <v>52</v>
       </c>
       <c r="L357">
@@ -28397,7 +28399,7 @@
       <c r="I358" t="s">
         <v>30</v>
       </c>
-      <c r="K358">
+      <c r="K358" s="5">
         <v>60</v>
       </c>
       <c r="L358">
@@ -28474,7 +28476,7 @@
       <c r="I359" t="s">
         <v>30</v>
       </c>
-      <c r="K359">
+      <c r="K359" s="5">
         <v>85</v>
       </c>
       <c r="L359">
@@ -28551,7 +28553,7 @@
       <c r="I360" t="s">
         <v>30</v>
       </c>
-      <c r="K360">
+      <c r="K360" s="5">
         <v>72</v>
       </c>
       <c r="L360">
@@ -28628,7 +28630,7 @@
       <c r="I361" t="s">
         <v>30</v>
       </c>
-      <c r="K361">
+      <c r="K361" s="5">
         <v>65</v>
       </c>
       <c r="L361">
@@ -28705,7 +28707,7 @@
       <c r="I362" t="s">
         <v>30</v>
       </c>
-      <c r="K362">
+      <c r="K362" s="5">
         <v>133</v>
       </c>
       <c r="L362">
@@ -28782,7 +28784,7 @@
       <c r="I363" t="s">
         <v>30</v>
       </c>
-      <c r="K363">
+      <c r="K363" s="5">
         <v>125</v>
       </c>
       <c r="L363">
@@ -28859,7 +28861,7 @@
       <c r="I364" t="s">
         <v>30</v>
       </c>
-      <c r="K364">
+      <c r="K364" s="5">
         <v>24</v>
       </c>
       <c r="L364">
@@ -28936,7 +28938,7 @@
       <c r="I365" t="s">
         <v>30</v>
       </c>
-      <c r="K365">
+      <c r="K365" s="5">
         <v>54</v>
       </c>
       <c r="L365">
@@ -29013,7 +29015,7 @@
       <c r="I366" t="s">
         <v>30</v>
       </c>
-      <c r="K366">
+      <c r="K366" s="5">
         <v>85</v>
       </c>
       <c r="L366">
@@ -29090,7 +29092,7 @@
       <c r="I367" t="s">
         <v>30</v>
       </c>
-      <c r="K367">
+      <c r="K367" s="5">
         <v>94</v>
       </c>
       <c r="L367">
@@ -29170,7 +29172,7 @@
       <c r="J368">
         <v>2</v>
       </c>
-      <c r="K368">
+      <c r="K368" s="5">
         <v>102</v>
       </c>
       <c r="L368">
@@ -29247,7 +29249,7 @@
       <c r="I369" t="s">
         <v>30</v>
       </c>
-      <c r="K369">
+      <c r="K369" s="5">
         <v>39</v>
       </c>
       <c r="L369">
@@ -29324,7 +29326,7 @@
       <c r="I370" t="s">
         <v>30</v>
       </c>
-      <c r="K370">
+      <c r="K370" s="5">
         <v>145</v>
       </c>
       <c r="L370">
@@ -29401,7 +29403,7 @@
       <c r="I371" t="s">
         <v>30</v>
       </c>
-      <c r="K371">
+      <c r="K371" s="5">
         <v>70</v>
       </c>
       <c r="L371">
@@ -29481,7 +29483,7 @@
       <c r="J372">
         <v>1</v>
       </c>
-      <c r="K372">
+      <c r="K372" s="5">
         <v>100</v>
       </c>
       <c r="L372">
@@ -29558,7 +29560,7 @@
       <c r="I373" t="s">
         <v>30</v>
       </c>
-      <c r="K373">
+      <c r="K373" s="5">
         <v>30</v>
       </c>
       <c r="L373">
@@ -29635,7 +29637,7 @@
       <c r="I374" t="s">
         <v>30</v>
       </c>
-      <c r="K374">
+      <c r="K374" s="5">
         <v>60</v>
       </c>
       <c r="L374">
@@ -29712,7 +29714,7 @@
       <c r="I375" t="s">
         <v>30</v>
       </c>
-      <c r="K375">
+      <c r="K375" s="5">
         <v>40</v>
       </c>
       <c r="L375">
@@ -29789,7 +29791,7 @@
       <c r="I376" t="s">
         <v>30</v>
       </c>
-      <c r="K376">
+      <c r="K376" s="5">
         <v>80</v>
       </c>
       <c r="L376">
@@ -29866,7 +29868,7 @@
       <c r="I377" t="s">
         <v>30</v>
       </c>
-      <c r="K377">
+      <c r="K377" s="5">
         <v>100</v>
       </c>
       <c r="L377">
@@ -29943,7 +29945,7 @@
       <c r="I378" t="s">
         <v>30</v>
       </c>
-      <c r="K378">
+      <c r="K378" s="5">
         <v>47</v>
       </c>
       <c r="L378">
@@ -30020,7 +30022,7 @@
       <c r="I379" t="s">
         <v>30</v>
       </c>
-      <c r="K379">
+      <c r="K379" s="5">
         <v>46</v>
       </c>
       <c r="L379">
@@ -30097,7 +30099,7 @@
       <c r="I380" t="s">
         <v>30</v>
       </c>
-      <c r="K380">
+      <c r="K380" s="5">
         <v>20</v>
       </c>
       <c r="L380">
@@ -30174,7 +30176,7 @@
       <c r="I381" t="s">
         <v>30</v>
       </c>
-      <c r="K381">
+      <c r="K381" s="5">
         <v>13</v>
       </c>
       <c r="L381">
@@ -30251,7 +30253,7 @@
       <c r="I382" t="s">
         <v>30</v>
       </c>
-      <c r="K382">
+      <c r="K382" s="5">
         <v>13</v>
       </c>
       <c r="L382">
@@ -30328,7 +30330,7 @@
       <c r="I383" t="s">
         <v>30</v>
       </c>
-      <c r="K383">
+      <c r="K383" s="5">
         <v>29</v>
       </c>
       <c r="L383">
@@ -30405,7 +30407,7 @@
       <c r="I384" t="s">
         <v>30</v>
       </c>
-      <c r="K384">
+      <c r="K384" s="5">
         <v>105</v>
       </c>
       <c r="L384">
@@ -30482,7 +30484,7 @@
       <c r="I385" t="s">
         <v>30</v>
       </c>
-      <c r="K385">
+      <c r="K385" s="5">
         <v>70</v>
       </c>
       <c r="L385">
@@ -30559,7 +30561,7 @@
       <c r="I386" t="s">
         <v>30</v>
       </c>
-      <c r="K386">
+      <c r="K386" s="5">
         <v>55</v>
       </c>
       <c r="L386">
@@ -30636,7 +30638,7 @@
       <c r="I387" t="s">
         <v>30</v>
       </c>
-      <c r="K387">
+      <c r="K387" s="5">
         <v>120</v>
       </c>
       <c r="L387">
@@ -30713,7 +30715,7 @@
       <c r="I388" t="s">
         <v>30</v>
       </c>
-      <c r="K388">
+      <c r="K388" s="5">
         <v>50</v>
       </c>
       <c r="L388">
@@ -30790,7 +30792,7 @@
       <c r="I389" t="s">
         <v>30</v>
       </c>
-      <c r="K389">
+      <c r="K389" s="5">
         <v>130</v>
       </c>
       <c r="L389">
@@ -30867,7 +30869,7 @@
       <c r="I390" t="s">
         <v>30</v>
       </c>
-      <c r="K390">
+      <c r="K390" s="5">
         <v>35</v>
       </c>
       <c r="L390">
@@ -30944,7 +30946,7 @@
       <c r="I391" t="s">
         <v>30</v>
       </c>
-      <c r="K391">
+      <c r="K391" s="5">
         <v>79</v>
       </c>
       <c r="L391">
@@ -31021,7 +31023,7 @@
       <c r="I392" t="s">
         <v>30</v>
       </c>
-      <c r="K392">
+      <c r="K392" s="5">
         <v>100</v>
       </c>
       <c r="L392">
@@ -31095,7 +31097,7 @@
       <c r="I393" t="s">
         <v>30</v>
       </c>
-      <c r="K393">
+      <c r="K393" s="5">
         <v>297</v>
       </c>
       <c r="L393">
@@ -31175,7 +31177,7 @@
       <c r="J394">
         <v>2</v>
       </c>
-      <c r="K394">
+      <c r="K394" s="5">
         <v>30</v>
       </c>
       <c r="L394">
@@ -31252,7 +31254,7 @@
       <c r="I395" t="s">
         <v>30</v>
       </c>
-      <c r="K395">
+      <c r="K395" s="5">
         <v>23</v>
       </c>
       <c r="L395">
@@ -31329,7 +31331,7 @@
       <c r="I396" t="s">
         <v>30</v>
       </c>
-      <c r="K396">
+      <c r="K396" s="5">
         <v>50</v>
       </c>
       <c r="L396">
@@ -31406,7 +31408,7 @@
       <c r="I397" t="s">
         <v>30</v>
       </c>
-      <c r="K397">
+      <c r="K397" s="5">
         <v>70</v>
       </c>
       <c r="L397">
@@ -31483,7 +31485,7 @@
       <c r="I398" t="s">
         <v>30</v>
       </c>
-      <c r="K398">
+      <c r="K398" s="5">
         <v>95</v>
       </c>
       <c r="L398">
@@ -31560,7 +31562,7 @@
       <c r="I399" t="s">
         <v>30</v>
       </c>
-      <c r="K399">
+      <c r="K399" s="5">
         <v>73</v>
       </c>
       <c r="L399">
@@ -31637,7 +31639,7 @@
       <c r="I400" t="s">
         <v>30</v>
       </c>
-      <c r="K400">
+      <c r="K400" s="5">
         <v>135</v>
       </c>
       <c r="L400">
@@ -31714,7 +31716,7 @@
       <c r="I401" t="s">
         <v>30</v>
       </c>
-      <c r="K401">
+      <c r="K401" s="5">
         <v>56</v>
       </c>
       <c r="L401">
@@ -31791,7 +31793,7 @@
       <c r="I402" t="s">
         <v>30</v>
       </c>
-      <c r="K402">
+      <c r="K402" s="5">
         <v>46</v>
       </c>
       <c r="L402">
@@ -31868,7 +31870,7 @@
       <c r="I403" t="s">
         <v>30</v>
       </c>
-      <c r="K403">
+      <c r="K403" s="5">
         <v>44</v>
       </c>
       <c r="L403">
@@ -31945,7 +31947,7 @@
       <c r="I404" t="s">
         <v>30</v>
       </c>
-      <c r="K404">
+      <c r="K404" s="5">
         <v>53</v>
       </c>
       <c r="L404">
@@ -32019,7 +32021,7 @@
       <c r="I405" t="s">
         <v>30</v>
       </c>
-      <c r="K405">
+      <c r="K405" s="5">
         <v>309</v>
       </c>
       <c r="L405">
@@ -32096,7 +32098,7 @@
       <c r="I406" t="s">
         <v>30</v>
       </c>
-      <c r="K406">
+      <c r="K406" s="5">
         <v>32</v>
       </c>
       <c r="L406">
@@ -32170,7 +32172,7 @@
       <c r="I407" t="s">
         <v>30</v>
       </c>
-      <c r="K407">
+      <c r="K407" s="5">
         <v>60</v>
       </c>
       <c r="L407">
@@ -32247,7 +32249,7 @@
       <c r="I408" t="s">
         <v>30</v>
       </c>
-      <c r="K408">
+      <c r="K408" s="5">
         <v>60</v>
       </c>
       <c r="L408">
@@ -32321,7 +32323,7 @@
       <c r="I409" t="s">
         <v>30</v>
       </c>
-      <c r="K409">
+      <c r="K409" s="5">
         <v>70</v>
       </c>
       <c r="L409">
@@ -32383,7 +32385,7 @@
       <c r="I410" t="s">
         <v>30</v>
       </c>
-      <c r="K410">
+      <c r="K410" s="5">
         <v>63</v>
       </c>
       <c r="L410">
@@ -32457,7 +32459,7 @@
       <c r="I411" t="s">
         <v>30</v>
       </c>
-      <c r="K411">
+      <c r="K411" s="5">
         <v>48</v>
       </c>
       <c r="L411">
@@ -32531,7 +32533,7 @@
       <c r="I412" t="s">
         <v>30</v>
       </c>
-      <c r="K412">
+      <c r="K412" s="5">
         <v>50</v>
       </c>
       <c r="L412">
@@ -32605,7 +32607,7 @@
       <c r="I413" t="s">
         <v>30</v>
       </c>
-      <c r="K413">
+      <c r="K413" s="5">
         <v>98</v>
       </c>
       <c r="L413">
@@ -32679,7 +32681,7 @@
       <c r="I414" t="s">
         <v>30</v>
       </c>
-      <c r="K414">
+      <c r="K414" s="5">
         <v>100</v>
       </c>
       <c r="L414">
@@ -32753,7 +32755,7 @@
       <c r="I415" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K415">
+      <c r="K415" s="5">
         <v>50</v>
       </c>
       <c r="L415">
@@ -32827,7 +32829,7 @@
       <c r="I416" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K416">
+      <c r="K416" s="5">
         <v>20</v>
       </c>
       <c r="L416">
@@ -32901,7 +32903,7 @@
       <c r="I417" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K417">
+      <c r="K417" s="5">
         <v>33</v>
       </c>
       <c r="L417">
@@ -32978,7 +32980,7 @@
       <c r="I418" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K418">
+      <c r="K418" s="5">
         <v>80</v>
       </c>
       <c r="L418">
@@ -33052,7 +33054,7 @@
       <c r="I419" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K419">
+      <c r="K419" s="5">
         <v>45</v>
       </c>
       <c r="L419">
@@ -33126,7 +33128,7 @@
       <c r="I420" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K420">
+      <c r="K420" s="5">
         <v>100</v>
       </c>
       <c r="L420">
@@ -33200,7 +33202,7 @@
       <c r="I421" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K421">
+      <c r="K421" s="5">
         <v>60</v>
       </c>
       <c r="L421">
@@ -33274,7 +33276,7 @@
       <c r="I422" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K422">
+      <c r="K422" s="5">
         <v>75</v>
       </c>
       <c r="L422">
@@ -33351,7 +33353,7 @@
       <c r="I423" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K423">
+      <c r="K423" s="5">
         <v>74</v>
       </c>
       <c r="L423">
@@ -33425,7 +33427,7 @@
       <c r="I424" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K424">
+      <c r="K424" s="5">
         <v>85</v>
       </c>
       <c r="L424">
@@ -33499,7 +33501,7 @@
       <c r="I425" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K425">
+      <c r="K425" s="5">
         <v>100</v>
       </c>
       <c r="L425">
@@ -33573,7 +33575,7 @@
       <c r="I426" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K426">
+      <c r="K426" s="5">
         <v>110</v>
       </c>
       <c r="L426">
@@ -33647,7 +33649,7 @@
       <c r="I427" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K427">
+      <c r="K427" s="5">
         <v>80</v>
       </c>
       <c r="L427">
@@ -33721,7 +33723,7 @@
       <c r="I428" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K428">
+      <c r="K428" s="5">
         <v>60</v>
       </c>
       <c r="L428">
@@ -33795,7 +33797,7 @@
       <c r="I429" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K429">
+      <c r="K429" s="5">
         <v>197</v>
       </c>
       <c r="L429">
@@ -33869,7 +33871,7 @@
       <c r="I430" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K430">
+      <c r="K430" s="5">
         <v>100</v>
       </c>
       <c r="L430">
@@ -33943,7 +33945,7 @@
       <c r="I431" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K431">
+      <c r="K431" s="5">
         <v>130</v>
       </c>
       <c r="L431">
@@ -34017,7 +34019,7 @@
       <c r="I432" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K432">
+      <c r="K432" s="5">
         <v>18</v>
       </c>
       <c r="L432">
@@ -34091,7 +34093,7 @@
       <c r="I433" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K433">
+      <c r="K433" s="5">
         <v>130</v>
       </c>
       <c r="L433">
@@ -34165,7 +34167,7 @@
       <c r="I434" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K434">
+      <c r="K434" s="5">
         <v>75</v>
       </c>
       <c r="L434">
@@ -34239,7 +34241,7 @@
       <c r="I435" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K435">
+      <c r="K435" s="5">
         <v>145</v>
       </c>
       <c r="L435">
@@ -34313,7 +34315,7 @@
       <c r="I436" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K436">
+      <c r="K436" s="5">
         <v>30</v>
       </c>
       <c r="L436">
@@ -34387,7 +34389,7 @@
       <c r="I437" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K437">
+      <c r="K437" s="5">
         <v>110</v>
       </c>
       <c r="L437">
@@ -34461,7 +34463,7 @@
       <c r="I438" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K438">
+      <c r="K438" s="5">
         <v>95</v>
       </c>
       <c r="L438">
@@ -34535,7 +34537,7 @@
       <c r="I439" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K439">
+      <c r="K439" s="5">
         <v>120</v>
       </c>
       <c r="L439">
@@ -34609,7 +34611,7 @@
       <c r="I440" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K440">
+      <c r="K440" s="5">
         <v>50</v>
       </c>
       <c r="L440">

</xml_diff>